<commit_message>
Feature : Adding new features in Province(#02)
</commit_message>
<xml_diff>
--- a/Book2.xlsx
+++ b/Book2.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ilola João\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ilola João\source\repos\LAB_APP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5771F3C9-6A8B-4710-9D56-6966F27CA6D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBAAD749-C97D-44EA-8C33-CD4FFC1CDEB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{91A32D49-347E-47BD-9C9E-DD4118A90A21}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
   <si>
     <t>nome</t>
   </si>
@@ -58,6 +58,12 @@
   </si>
   <si>
     <t>Benguela</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LV </t>
+  </si>
+  <si>
+    <t>escolalv@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -420,10 +426,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89F1BF9E-BBC9-48E1-9AEC-222687C1D389}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -489,11 +495,26 @@
         <v>10</v>
       </c>
     </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5">
+        <v>12</v>
+      </c>
+      <c r="D5" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{B9259908-3DA5-4BFE-A07C-90930163AC59}"/>
     <hyperlink ref="B3" r:id="rId2" xr:uid="{DA3DFBF1-7FB9-4377-89CC-23E7F67F8FE6}"/>
     <hyperlink ref="B4" r:id="rId3" xr:uid="{F472AF7D-2359-40DB-95F7-24C8F33F0D4B}"/>
+    <hyperlink ref="B5" r:id="rId4" xr:uid="{98D0D9CD-9C6C-4172-BD87-50858D72C7F9}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>